<commit_message>
Add requirements.txt to typeIII analysis. Correct Chemicalize submission files and user map.
</commit_message>
<xml_diff>
--- a/predictions/20181203_Chemicalize_pKa_predictions/comparison_of_chemicalize_versions.xlsx
+++ b/predictions/20181203_Chemicalize_pKa_predictions/comparison_of_chemicalize_versions.xlsx
@@ -4,10 +4,11 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26004"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="14560" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="14700" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="All" sheetId="1" r:id="rId1"/>
+    <sheet name="SM18" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="140000" concurrentCalc="0"/>
   <extLst>
@@ -19,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="37">
   <si>
     <t>SM01</t>
   </si>
@@ -102,10 +103,34 @@
     <t>Chemicalize-1</t>
   </si>
   <si>
-    <t>Difference</t>
-  </si>
-  <si>
-    <t>Experimental pKa</t>
+    <t>Difference between versions</t>
+  </si>
+  <si>
+    <t>Closest Exp Match</t>
+  </si>
+  <si>
+    <t>Match prediction to experiment</t>
+  </si>
+  <si>
+    <t>Match experiment to prediction</t>
+  </si>
+  <si>
+    <t>Unordered experimental values</t>
+  </si>
+  <si>
+    <t>RMSE</t>
+  </si>
+  <si>
+    <t>Prediction difference between versions</t>
+  </si>
+  <si>
+    <t>Pred - Exp</t>
+  </si>
+  <si>
+    <t>Chemicalize-1 predictions</t>
+  </si>
+  <si>
+    <t>Chemicalize-2 predictions</t>
   </si>
 </sst>
 </file>
@@ -137,7 +162,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -147,6 +172,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.14999847407452621"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -160,18 +191,38 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="3">
+  <cellStyleXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="3">
+  <cellStyles count="11">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -183,13 +234,13 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>6</xdr:col>
+      <xdr:col>10</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>1</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>15</xdr:col>
+      <xdr:col>19</xdr:col>
       <xdr:colOff>800100</xdr:colOff>
       <xdr:row>26</xdr:row>
       <xdr:rowOff>63500</xdr:rowOff>
@@ -221,13 +272,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>6</xdr:col>
+      <xdr:col>10</xdr:col>
       <xdr:colOff>25400</xdr:colOff>
       <xdr:row>27</xdr:row>
       <xdr:rowOff>101599</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>15</xdr:col>
+      <xdr:col>19</xdr:col>
       <xdr:colOff>774700</xdr:colOff>
       <xdr:row>52</xdr:row>
       <xdr:rowOff>150158</xdr:rowOff>
@@ -248,6 +299,87 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="5232400" y="5245099"/>
+          <a:ext cx="8178800" cy="4811059"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>23</xdr:col>
+      <xdr:colOff>800100</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>63500</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="9512300" y="190500"/>
+          <a:ext cx="8229600" cy="4826000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>25400</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>23</xdr:col>
+      <xdr:colOff>774700</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>48559</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Picture 2"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="9537700" y="5245099"/>
           <a:ext cx="8178800" cy="4811059"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -582,18 +714,24 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E55"/>
+  <dimension ref="A1:G55"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="R39" sqref="R39"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
-    <col min="2" max="3" width="12.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.5" customWidth="1"/>
+    <col min="4" max="4" width="12.5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.5" customWidth="1"/>
+    <col min="6" max="6" width="24.5" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.5" bestFit="1" customWidth="1"/>
+    <col min="8" max="10" width="8" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:6">
       <c r="A1" t="s">
         <v>24</v>
       </c>
@@ -601,830 +739,833 @@
         <v>26</v>
       </c>
       <c r="C1" t="s">
+        <v>28</v>
+      </c>
+      <c r="D1" t="s">
         <v>25</v>
-      </c>
-      <c r="D1" t="s">
-        <v>27</v>
       </c>
       <c r="E1" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="2" spans="1:5">
+      <c r="F1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6">
       <c r="A2" t="s">
         <v>0</v>
       </c>
       <c r="B2">
         <v>9.44</v>
       </c>
-      <c r="C2">
+      <c r="D2">
         <v>9.44</v>
       </c>
-      <c r="D2">
-        <f>C2-B2</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5">
+      <c r="F2">
+        <f>D2-B2</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6">
       <c r="A3" t="s">
         <v>0</v>
       </c>
       <c r="B3">
         <v>14.71</v>
       </c>
-      <c r="C3">
+      <c r="D3">
         <v>14.71</v>
       </c>
-      <c r="D3">
-        <f t="shared" ref="D3:D55" si="0">C3-B3</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5">
+      <c r="F3">
+        <f t="shared" ref="F3:F55" si="0">D3-B3</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6">
       <c r="A4" t="s">
         <v>1</v>
       </c>
       <c r="B4">
         <v>4.01</v>
       </c>
-      <c r="C4">
+      <c r="D4">
         <v>4.01</v>
       </c>
-      <c r="D4">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5">
+      <c r="F4">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6">
       <c r="A5" t="s">
         <v>1</v>
       </c>
       <c r="B5">
         <v>15.64</v>
       </c>
-      <c r="C5">
+      <c r="D5">
         <v>15.64</v>
       </c>
-      <c r="D5">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5">
+      <c r="F5">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6">
       <c r="A6" t="s">
         <v>2</v>
       </c>
       <c r="B6">
         <v>-0.31</v>
       </c>
-      <c r="C6">
+      <c r="D6">
         <v>-0.31</v>
       </c>
-      <c r="D6">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5">
+      <c r="F6">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6">
       <c r="A7" t="s">
         <v>2</v>
       </c>
       <c r="B7">
         <v>7.68</v>
       </c>
-      <c r="C7">
+      <c r="D7">
         <v>7.68</v>
       </c>
-      <c r="D7">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5">
+      <c r="F7">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6">
       <c r="A8" t="s">
         <v>3</v>
       </c>
       <c r="B8">
         <v>-1.61</v>
       </c>
-      <c r="C8">
+      <c r="D8">
         <v>-1.61</v>
       </c>
-      <c r="D8">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5">
+      <c r="F8">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6">
       <c r="A9" t="s">
         <v>3</v>
       </c>
       <c r="B9">
         <v>4.83</v>
       </c>
-      <c r="C9">
+      <c r="D9">
         <v>4.83</v>
       </c>
-      <c r="D9">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5">
+      <c r="F9">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6">
       <c r="A10" t="s">
         <v>4</v>
       </c>
       <c r="B10">
         <v>4.1900000000000004</v>
       </c>
-      <c r="C10">
+      <c r="D10">
         <v>4.1900000000000004</v>
       </c>
-      <c r="D10">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5">
+      <c r="F10">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6">
       <c r="A11" t="s">
         <v>4</v>
       </c>
       <c r="B11">
         <v>13.53</v>
       </c>
-      <c r="C11">
+      <c r="D11">
         <v>13.53</v>
       </c>
-      <c r="D11">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5">
+      <c r="F11">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6">
       <c r="A12" t="s">
         <v>5</v>
       </c>
       <c r="B12">
         <v>1.83</v>
       </c>
-      <c r="C12">
+      <c r="D12">
         <v>1.83</v>
       </c>
-      <c r="D12">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5">
+      <c r="F12">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6">
       <c r="A13" t="s">
         <v>5</v>
       </c>
       <c r="B13">
         <v>3.42</v>
       </c>
-      <c r="C13">
+      <c r="D13">
         <v>3.42</v>
       </c>
-      <c r="D13">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5">
+      <c r="F13">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6">
       <c r="A14" t="s">
         <v>5</v>
       </c>
       <c r="B14">
         <v>13.85</v>
       </c>
-      <c r="C14">
+      <c r="D14">
         <v>13.85</v>
       </c>
-      <c r="D14">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5">
+      <c r="F14">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6">
       <c r="A15" t="s">
         <v>6</v>
       </c>
       <c r="B15">
         <v>-1.61</v>
       </c>
-      <c r="C15">
+      <c r="D15">
         <v>-1.61</v>
       </c>
-      <c r="D15">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5">
+      <c r="F15">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6">
       <c r="A16" t="s">
         <v>6</v>
       </c>
       <c r="B16">
         <v>4.83</v>
       </c>
-      <c r="C16">
+      <c r="D16">
         <v>4.83</v>
       </c>
-      <c r="D16">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4">
+      <c r="F16">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6">
       <c r="A17" t="s">
         <v>7</v>
       </c>
       <c r="B17">
         <v>-1.64</v>
       </c>
-      <c r="C17">
+      <c r="D17">
         <v>-1.64</v>
       </c>
-      <c r="D17">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4">
+      <c r="F17">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6">
       <c r="A18" t="s">
         <v>7</v>
       </c>
       <c r="B18">
         <v>4.2</v>
       </c>
-      <c r="C18">
+      <c r="D18">
         <v>4.2</v>
       </c>
-      <c r="D18">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4">
+      <c r="F18">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6">
       <c r="A19" t="s">
         <v>7</v>
       </c>
       <c r="B19">
         <v>13.72</v>
       </c>
-      <c r="C19">
+      <c r="D19">
         <v>13.72</v>
       </c>
-      <c r="D19">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4">
+      <c r="F19">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6">
       <c r="A20" t="s">
         <v>8</v>
       </c>
       <c r="B20">
         <v>4</v>
       </c>
-      <c r="C20">
+      <c r="D20">
         <v>4</v>
       </c>
-      <c r="D20">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4">
+      <c r="F20">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6">
       <c r="A21" t="s">
         <v>8</v>
       </c>
       <c r="B21">
         <v>15.62</v>
       </c>
-      <c r="C21">
+      <c r="D21">
         <v>15.62</v>
       </c>
-      <c r="D21">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4">
+      <c r="F21">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6">
       <c r="A22" t="s">
         <v>9</v>
       </c>
       <c r="B22">
         <v>-1.37</v>
       </c>
-      <c r="C22">
+      <c r="D22">
         <v>-1.37</v>
       </c>
-      <c r="D22">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4">
+      <c r="F22">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6">
       <c r="A23" t="s">
         <v>9</v>
       </c>
       <c r="B23">
         <v>-0.56999999999999995</v>
       </c>
-      <c r="C23">
+      <c r="D23">
         <v>-0.56999999999999995</v>
       </c>
-      <c r="D23">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4">
+      <c r="F23">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6">
       <c r="A24" t="s">
         <v>9</v>
       </c>
       <c r="B24">
         <v>7.77</v>
       </c>
-      <c r="C24">
+      <c r="D24">
         <v>7.77</v>
       </c>
-      <c r="D24">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4">
+      <c r="F24">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6">
       <c r="A25" t="s">
         <v>9</v>
       </c>
       <c r="B25">
         <v>15.06</v>
       </c>
-      <c r="C25">
+      <c r="D25">
         <v>15.06</v>
       </c>
-      <c r="D25">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4">
+      <c r="F25">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6">
       <c r="A26" t="s">
         <v>10</v>
       </c>
       <c r="B26">
         <v>-0.54</v>
       </c>
-      <c r="C26">
+      <c r="D26">
         <v>-0.54</v>
       </c>
-      <c r="D26">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4">
+      <c r="F26">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6">
       <c r="A27" t="s">
         <v>10</v>
       </c>
       <c r="B27">
         <v>3.42</v>
       </c>
-      <c r="C27">
+      <c r="D27">
         <v>3.42</v>
       </c>
-      <c r="D27">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4">
+      <c r="F27">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6">
       <c r="A28" t="s">
         <v>11</v>
       </c>
       <c r="B28">
         <v>4.01</v>
       </c>
-      <c r="C28">
+      <c r="D28">
         <v>4.01</v>
       </c>
-      <c r="D28">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="29" spans="1:4">
+      <c r="F28">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6">
       <c r="A29" t="s">
         <v>11</v>
       </c>
       <c r="B29">
         <v>15.6</v>
       </c>
-      <c r="C29">
+      <c r="D29">
         <v>15.6</v>
       </c>
-      <c r="D29">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="30" spans="1:4">
+      <c r="F29">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6">
       <c r="A30" t="s">
         <v>12</v>
       </c>
       <c r="B30">
         <v>-1.4</v>
       </c>
-      <c r="C30">
+      <c r="D30">
         <v>-1.4</v>
       </c>
-      <c r="D30">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="31" spans="1:4">
+      <c r="F30">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6">
       <c r="A31" t="s">
         <v>12</v>
       </c>
       <c r="B31">
         <v>4.68</v>
       </c>
-      <c r="C31">
+      <c r="D31">
         <v>4.68</v>
       </c>
-      <c r="D31">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="32" spans="1:4">
+      <c r="F31">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6">
       <c r="A32" t="s">
         <v>13</v>
       </c>
       <c r="B32">
         <v>0.93</v>
       </c>
-      <c r="C32">
+      <c r="D32">
         <v>0.93</v>
       </c>
-      <c r="D32">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="33" spans="1:5">
+      <c r="F32">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7">
       <c r="A33" t="s">
         <v>13</v>
       </c>
       <c r="B33">
         <v>6.4</v>
       </c>
-      <c r="C33">
+      <c r="D33">
         <v>6.4</v>
       </c>
-      <c r="D33">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="34" spans="1:5">
+      <c r="F33">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7">
       <c r="A34" t="s">
         <v>14</v>
       </c>
       <c r="B34">
         <v>4.91</v>
       </c>
-      <c r="C34">
+      <c r="D34">
         <v>4.91</v>
       </c>
-      <c r="D34">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="35" spans="1:5">
+      <c r="F34">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7">
       <c r="A35" t="s">
         <v>14</v>
       </c>
       <c r="B35">
         <v>10.64</v>
       </c>
-      <c r="C35">
+      <c r="D35">
         <v>10.64</v>
       </c>
-      <c r="D35">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="36" spans="1:5">
+      <c r="F35">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7">
       <c r="A36" t="s">
         <v>15</v>
       </c>
       <c r="B36">
         <v>5.61</v>
       </c>
-      <c r="C36">
+      <c r="D36">
         <v>5.61</v>
       </c>
-      <c r="D36">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="37" spans="1:5">
+      <c r="F36">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7">
       <c r="A37" t="s">
         <v>15</v>
       </c>
       <c r="B37">
         <v>13.98</v>
       </c>
-      <c r="C37">
+      <c r="D37">
         <v>13.98</v>
       </c>
-      <c r="D37">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="38" spans="1:5">
+      <c r="F37">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7">
       <c r="A38" t="s">
         <v>16</v>
       </c>
       <c r="B38">
         <v>2.48</v>
       </c>
-      <c r="C38">
+      <c r="D38">
         <v>2.48</v>
       </c>
-      <c r="D38">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="39" spans="1:5">
+      <c r="F38">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7">
       <c r="A39" t="s">
         <v>17</v>
       </c>
       <c r="B39">
         <v>0.22</v>
       </c>
-      <c r="C39">
+      <c r="D39">
         <v>0.2</v>
       </c>
-      <c r="D39" s="1">
+      <c r="F39" s="1">
         <f t="shared" si="0"/>
         <v>-1.999999999999999E-2</v>
       </c>
     </row>
-    <row r="40" spans="1:5">
+    <row r="40" spans="1:7">
       <c r="A40" t="s">
         <v>17</v>
       </c>
       <c r="B40">
         <v>5.4</v>
       </c>
-      <c r="C40">
+      <c r="D40">
         <v>1.55</v>
       </c>
-      <c r="D40" s="1">
+      <c r="F40" s="1">
         <f t="shared" si="0"/>
         <v>-3.8500000000000005</v>
       </c>
-      <c r="E40">
+      <c r="G40">
         <v>2.15</v>
       </c>
     </row>
-    <row r="41" spans="1:5">
+    <row r="41" spans="1:7">
       <c r="A41" t="s">
         <v>17</v>
       </c>
       <c r="B41">
         <v>8.0399999999999991</v>
       </c>
-      <c r="C41">
+      <c r="D41">
         <v>8.0399999999999991</v>
       </c>
-      <c r="D41" s="1">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="E41">
+      <c r="F41" s="1">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="G41">
         <v>9.58</v>
       </c>
     </row>
-    <row r="42" spans="1:5">
+    <row r="42" spans="1:7">
       <c r="A42" t="s">
         <v>17</v>
       </c>
       <c r="B42">
         <v>9.93</v>
       </c>
-      <c r="C42">
+      <c r="D42">
         <v>12.54</v>
       </c>
-      <c r="D42" s="1">
+      <c r="F42" s="1">
         <f t="shared" si="0"/>
         <v>2.6099999999999994</v>
       </c>
-      <c r="E42">
+      <c r="G42">
         <v>11.02</v>
       </c>
     </row>
-    <row r="43" spans="1:5">
+    <row r="43" spans="1:7">
       <c r="A43" t="s">
         <v>18</v>
       </c>
       <c r="B43">
         <v>-0.42</v>
       </c>
-      <c r="C43">
+      <c r="D43">
         <v>-0.42</v>
       </c>
-      <c r="D43">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="44" spans="1:5">
+      <c r="F43">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7">
       <c r="A44" t="s">
         <v>18</v>
       </c>
       <c r="B44">
         <v>7.89</v>
       </c>
-      <c r="C44">
+      <c r="D44">
         <v>7.89</v>
       </c>
-      <c r="D44">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="45" spans="1:5">
+      <c r="F44">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="45" spans="1:7">
       <c r="A45" t="s">
         <v>19</v>
       </c>
       <c r="B45">
         <v>7.2</v>
       </c>
-      <c r="C45">
+      <c r="D45">
         <v>7.2</v>
       </c>
-      <c r="D45">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="46" spans="1:5">
+      <c r="F45">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="46" spans="1:7">
       <c r="A46" t="s">
         <v>20</v>
       </c>
       <c r="B46">
         <v>1.95</v>
       </c>
-      <c r="C46">
+      <c r="D46">
         <v>1.95</v>
       </c>
-      <c r="D46">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="47" spans="1:5">
+      <c r="F46">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="47" spans="1:7">
       <c r="A47" t="s">
         <v>20</v>
       </c>
       <c r="B47">
         <v>13.32</v>
       </c>
-      <c r="C47">
+      <c r="D47">
         <v>13.32</v>
       </c>
-      <c r="D47">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="48" spans="1:5">
+      <c r="F47">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="48" spans="1:7">
       <c r="A48" t="s">
         <v>20</v>
       </c>
       <c r="B48">
         <v>14.72</v>
       </c>
-      <c r="C48">
+      <c r="D48">
         <v>14.72</v>
       </c>
-      <c r="D48">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="49" spans="1:4">
+      <c r="F48">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6">
       <c r="A49" t="s">
         <v>21</v>
       </c>
       <c r="B49">
         <v>3.34</v>
       </c>
-      <c r="C49">
+      <c r="D49">
         <v>3.34</v>
       </c>
-      <c r="D49">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="50" spans="1:4">
+      <c r="F49">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6">
       <c r="A50" t="s">
         <v>21</v>
       </c>
       <c r="B50">
         <v>7.39</v>
       </c>
-      <c r="C50">
+      <c r="D50">
         <v>7.39</v>
       </c>
-      <c r="D50">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="51" spans="1:4">
+      <c r="F50">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6">
       <c r="A51" t="s">
         <v>22</v>
       </c>
       <c r="B51">
         <v>5.0199999999999996</v>
       </c>
-      <c r="C51">
+      <c r="D51">
         <v>5.0199999999999996</v>
       </c>
-      <c r="D51">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="52" spans="1:4">
+      <c r="F51">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6">
       <c r="A52" t="s">
         <v>22</v>
       </c>
       <c r="B52">
         <v>12.45</v>
       </c>
-      <c r="C52">
+      <c r="D52">
         <v>12.45</v>
       </c>
-      <c r="D52">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="53" spans="1:4">
+      <c r="F52">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6">
       <c r="A53" t="s">
         <v>22</v>
       </c>
       <c r="B53">
         <v>15.88</v>
       </c>
-      <c r="C53">
+      <c r="D53">
         <v>15.88</v>
       </c>
-      <c r="D53">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="54" spans="1:4">
+      <c r="F53">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="54" spans="1:6">
       <c r="A54" t="s">
         <v>23</v>
       </c>
       <c r="B54">
         <v>3.09</v>
       </c>
-      <c r="C54">
+      <c r="D54">
         <v>3.09</v>
       </c>
-      <c r="D54">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="55" spans="1:4">
+      <c r="F54">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="55" spans="1:6">
       <c r="A55" t="s">
         <v>23</v>
       </c>
       <c r="B55">
         <v>15.59</v>
       </c>
-      <c r="C55">
+      <c r="D55">
         <v>15.59</v>
       </c>
-      <c r="D55">
+      <c r="F55">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -1439,4 +1580,329 @@
     </ext>
   </extLst>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:K11"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E19" sqref="E19"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="2" max="2" width="12.5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.1640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.1640625" customWidth="1"/>
+    <col min="6" max="6" width="12.5" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="16.1640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="9" width="16.1640625" customWidth="1"/>
+    <col min="10" max="10" width="33.1640625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="27" bestFit="1" customWidth="1"/>
+    <col min="12" max="14" width="8" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11">
+      <c r="A1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="C1" t="s">
+        <v>28</v>
+      </c>
+      <c r="D1" t="s">
+        <v>34</v>
+      </c>
+      <c r="E1" t="s">
+        <v>32</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="G1" t="s">
+        <v>28</v>
+      </c>
+      <c r="H1" t="s">
+        <v>34</v>
+      </c>
+      <c r="I1" t="s">
+        <v>32</v>
+      </c>
+      <c r="J1" t="s">
+        <v>33</v>
+      </c>
+      <c r="K1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11">
+      <c r="A2" t="s">
+        <v>30</v>
+      </c>
+      <c r="B2" s="3"/>
+      <c r="F2" s="3"/>
+    </row>
+    <row r="3" spans="1:11">
+      <c r="A3" t="s">
+        <v>17</v>
+      </c>
+      <c r="B3" s="3">
+        <v>0.22</v>
+      </c>
+      <c r="C3">
+        <v>2.15</v>
+      </c>
+      <c r="D3">
+        <f>B3-C3</f>
+        <v>-1.93</v>
+      </c>
+      <c r="E3" s="2">
+        <f xml:space="preserve"> SQRT(SUMSQ(D3:D6)/COUNTA(D3:D6))</f>
+        <v>1.3869751259485512</v>
+      </c>
+      <c r="F3" s="3">
+        <v>0.2</v>
+      </c>
+      <c r="I3" s="2">
+        <f xml:space="preserve"> SQRT(SUMSQ(H3:H6)/COUNTA(H3:H6))</f>
+        <v>1.2575107686748985</v>
+      </c>
+      <c r="J3" s="1">
+        <f>F3-B3</f>
+        <v>-1.999999999999999E-2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11">
+      <c r="A4" t="s">
+        <v>17</v>
+      </c>
+      <c r="B4" s="3">
+        <v>5.4</v>
+      </c>
+      <c r="E4" s="2"/>
+      <c r="F4" s="3">
+        <v>1.55</v>
+      </c>
+      <c r="G4">
+        <v>2.15</v>
+      </c>
+      <c r="H4">
+        <f t="shared" ref="H4:H11" si="0">F4-G4</f>
+        <v>-0.59999999999999987</v>
+      </c>
+      <c r="I4" s="2"/>
+      <c r="J4" s="1">
+        <f>F4-B4</f>
+        <v>-3.8500000000000005</v>
+      </c>
+      <c r="K4">
+        <v>2.15</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11">
+      <c r="A5" t="s">
+        <v>17</v>
+      </c>
+      <c r="B5" s="3">
+        <v>8.0399999999999991</v>
+      </c>
+      <c r="E5" s="2"/>
+      <c r="F5" s="3">
+        <v>8.0399999999999991</v>
+      </c>
+      <c r="G5">
+        <v>9.48</v>
+      </c>
+      <c r="H5">
+        <f t="shared" si="0"/>
+        <v>-1.4400000000000013</v>
+      </c>
+      <c r="I5" s="2"/>
+      <c r="J5" s="1">
+        <f>F5-B5</f>
+        <v>0</v>
+      </c>
+      <c r="K5">
+        <v>9.58</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11">
+      <c r="A6" t="s">
+        <v>17</v>
+      </c>
+      <c r="B6" s="3">
+        <v>9.93</v>
+      </c>
+      <c r="C6">
+        <v>9.58</v>
+      </c>
+      <c r="D6">
+        <f t="shared" ref="D6:D11" si="1">B6-C6</f>
+        <v>0.34999999999999964</v>
+      </c>
+      <c r="E6" s="2"/>
+      <c r="F6" s="3">
+        <v>12.54</v>
+      </c>
+      <c r="G6">
+        <v>11.02</v>
+      </c>
+      <c r="H6">
+        <f t="shared" si="0"/>
+        <v>1.5199999999999996</v>
+      </c>
+      <c r="I6" s="2"/>
+      <c r="J6" s="1">
+        <f>F6-B6</f>
+        <v>2.6099999999999994</v>
+      </c>
+      <c r="K6">
+        <v>11.02</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11">
+      <c r="A7" t="s">
+        <v>29</v>
+      </c>
+      <c r="B7" s="3"/>
+      <c r="F7" s="3"/>
+    </row>
+    <row r="8" spans="1:11">
+      <c r="A8" t="s">
+        <v>17</v>
+      </c>
+      <c r="B8" s="3">
+        <v>0.22</v>
+      </c>
+      <c r="C8">
+        <v>2.15</v>
+      </c>
+      <c r="D8">
+        <f t="shared" si="1"/>
+        <v>-1.93</v>
+      </c>
+      <c r="E8" s="2">
+        <f xml:space="preserve"> SQRT(SUMSQ(D8:D11)/COUNTA(D8:D11))</f>
+        <v>1.3869751259485512</v>
+      </c>
+      <c r="F8" s="3">
+        <v>0.2</v>
+      </c>
+      <c r="I8" s="2">
+        <f xml:space="preserve"> SQRT(SUMSQ(H8:H11)/COUNTA(H8:H11))</f>
+        <v>1.2964052864234499</v>
+      </c>
+      <c r="J8" s="1">
+        <f>F8-B8</f>
+        <v>-1.999999999999999E-2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11">
+      <c r="A9" t="s">
+        <v>17</v>
+      </c>
+      <c r="B9" s="3">
+        <v>5.4</v>
+      </c>
+      <c r="E9" s="2"/>
+      <c r="F9" s="3">
+        <v>1.55</v>
+      </c>
+      <c r="G9">
+        <v>2.15</v>
+      </c>
+      <c r="H9">
+        <f t="shared" si="0"/>
+        <v>-0.59999999999999987</v>
+      </c>
+      <c r="I9" s="2"/>
+      <c r="J9" s="1">
+        <f>F9-B9</f>
+        <v>-3.8500000000000005</v>
+      </c>
+      <c r="K9">
+        <v>2.15</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11">
+      <c r="A10" t="s">
+        <v>17</v>
+      </c>
+      <c r="B10" s="3">
+        <v>8.0399999999999991</v>
+      </c>
+      <c r="E10" s="2"/>
+      <c r="F10" s="3">
+        <v>8.0399999999999991</v>
+      </c>
+      <c r="G10">
+        <v>9.58</v>
+      </c>
+      <c r="H10">
+        <f t="shared" si="0"/>
+        <v>-1.5400000000000009</v>
+      </c>
+      <c r="I10" s="2"/>
+      <c r="J10" s="1">
+        <f>F10-B10</f>
+        <v>0</v>
+      </c>
+      <c r="K10">
+        <v>9.58</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11">
+      <c r="A11" t="s">
+        <v>17</v>
+      </c>
+      <c r="B11" s="3">
+        <v>9.93</v>
+      </c>
+      <c r="C11">
+        <v>9.58</v>
+      </c>
+      <c r="D11">
+        <f t="shared" si="1"/>
+        <v>0.34999999999999964</v>
+      </c>
+      <c r="E11" s="2"/>
+      <c r="F11" s="3">
+        <v>12.54</v>
+      </c>
+      <c r="G11">
+        <v>11.02</v>
+      </c>
+      <c r="H11">
+        <f t="shared" si="0"/>
+        <v>1.5199999999999996</v>
+      </c>
+      <c r="I11" s="2"/>
+      <c r="J11" s="1">
+        <f>F11-B11</f>
+        <v>2.6099999999999994</v>
+      </c>
+      <c r="K11">
+        <v>11.02</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="4">
+    <mergeCell ref="E3:E6"/>
+    <mergeCell ref="E8:E11"/>
+    <mergeCell ref="I3:I6"/>
+    <mergeCell ref="I8:I11"/>
+  </mergeCells>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <drawing r:id="rId1"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
 </file>
</xml_diff>